<commit_message>
bank list updated, new models
</commit_message>
<xml_diff>
--- a/data/BankByDC.xlsx
+++ b/data/BankByDC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmz/Documents/WNE/Lic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB194EF4-AE99-5C47-A394-D1A31C9C9A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7823306-3063-3D44-9658-52625AEC3954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1120" windowWidth="27640" windowHeight="15380" xr2:uid="{546FC666-7022-2643-A28A-8C7A50C142F8}"/>
+    <workbookView xWindow="16740" yWindow="-20860" windowWidth="27640" windowHeight="15400" xr2:uid="{546FC666-7022-2643-A28A-8C7A50C142F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="218">
   <si>
     <t>BG Bank A/S</t>
   </si>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EED924B-AB36-B64A-9F03-43D3FB40726C}">
   <dimension ref="A1:B213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="141" workbookViewId="0">
-      <selection activeCell="D154" sqref="D154"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="141" workbookViewId="0">
+      <selection activeCell="A178" sqref="A178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1108,177 +1108,255 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>142</v>
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>137</v>
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>176</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>171</v>
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>170</v>
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>96</v>
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>100</v>
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>153</v>
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B18" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>197</v>
+        <v>176</v>
+      </c>
+      <c r="B19" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>23</v>
+        <v>201</v>
+      </c>
+      <c r="B20" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>109</v>
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>0</v>
+        <v>166</v>
+      </c>
+      <c r="B22" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>117</v>
+        <v>97</v>
+      </c>
+      <c r="B23" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>58</v>
+        <v>121</v>
+      </c>
+      <c r="B24" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>158</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>172</v>
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>39</v>
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>93</v>
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>68</v>
+        <v>40</v>
+      </c>
+      <c r="B29" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>200</v>
+      <c r="A30" t="s">
+        <v>205</v>
+      </c>
+      <c r="B30" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>196</v>
+        <v>202</v>
+      </c>
+      <c r="B31" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>66</v>
+        <v>98</v>
+      </c>
+      <c r="B32" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>201</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
         <v>213</v>
@@ -1286,7 +1364,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
         <v>213</v>
@@ -1294,117 +1372,159 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>89</v>
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>146</v>
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>112</v>
+        <v>55</v>
+      </c>
+      <c r="B38" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="B39" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>49</v>
+      <c r="A40" t="s">
+        <v>216</v>
       </c>
       <c r="B40" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>123</v>
+        <v>142</v>
+      </c>
+      <c r="B42" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>71</v>
+        <v>100</v>
+      </c>
+      <c r="B43" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>139</v>
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>173</v>
+        <v>106</v>
+      </c>
+      <c r="B45" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>74</v>
+        <v>195</v>
+      </c>
+      <c r="B46" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>43</v>
+        <v>9</v>
+      </c>
+      <c r="B47" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>188</v>
+        <v>154</v>
+      </c>
+      <c r="B48" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>199</v>
+        <v>103</v>
       </c>
       <c r="B49" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>206</v>
+      <c r="A50" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B50" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>106</v>
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>161</v>
+        <v>56</v>
+      </c>
+      <c r="B52" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>78</v>
+        <v>183</v>
+      </c>
+      <c r="B53" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>166</v>
+        <v>20</v>
       </c>
       <c r="B54" t="s">
         <v>213</v>
@@ -1412,946 +1532,898 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>195</v>
+        <v>147</v>
+      </c>
+      <c r="B55" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>198</v>
+        <v>84</v>
+      </c>
+      <c r="B56" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="B57" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>6</v>
+      <c r="A58" t="s">
+        <v>210</v>
+      </c>
+      <c r="B58" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
+      </c>
+      <c r="B59" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>76</v>
+        <v>22</v>
+      </c>
+      <c r="B60" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>101</v>
+      <c r="A61" t="s">
+        <v>206</v>
+      </c>
+      <c r="B61" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>107</v>
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>163</v>
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="B64" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>97</v>
+        <v>28</v>
       </c>
       <c r="B65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="B66" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B67" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
+      </c>
+      <c r="B68" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>184</v>
+        <v>95</v>
+      </c>
+      <c r="B69" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>132</v>
+      <c r="A70" t="s">
+        <v>203</v>
+      </c>
+      <c r="B70" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>152</v>
+        <v>88</v>
+      </c>
+      <c r="B72" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>111</v>
+        <v>75</v>
+      </c>
+      <c r="B74" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>128</v>
+        <v>157</v>
+      </c>
+      <c r="B75" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
-        <v>103</v>
+      <c r="A76" t="s">
+        <v>204</v>
+      </c>
+      <c r="B76" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="B77" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>143</v>
+        <v>2</v>
+      </c>
+      <c r="B78" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>114</v>
+        <v>199</v>
+      </c>
+      <c r="B79" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="2" t="s">
-        <v>118</v>
+      <c r="A80" t="s">
+        <v>207</v>
+      </c>
+      <c r="B80" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>175</v>
+        <v>1</v>
+      </c>
+      <c r="B81" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>155</v>
+        <v>186</v>
+      </c>
+      <c r="B82" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>127</v>
+        <v>189</v>
+      </c>
+      <c r="B83" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>53</v>
+        <v>185</v>
       </c>
       <c r="B84" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>126</v>
+        <v>91</v>
+      </c>
+      <c r="B85" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>148</v>
+        <v>187</v>
+      </c>
+      <c r="B86" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>180</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>181</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>174</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>72</v>
+        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>80</v>
+        <v>153</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B94" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B95" t="s">
-        <v>212</v>
+        <v>23</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>207</v>
-      </c>
-      <c r="B97" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="2" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B99" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B100" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B101" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="2" t="s">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="2" t="s">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="2" t="s">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="2" t="s">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="2" t="s">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="2" t="s">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B108" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>205</v>
-      </c>
-      <c r="B109" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="2" t="s">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B111" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B113" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B114" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="2" t="s">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="2" t="s">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="2" t="s">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B118" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="2" t="s">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="2" t="s">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="2" t="s">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B123" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B124" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B125" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B126" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="2" t="s">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B128" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="2" t="s">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="2" t="s">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="2" t="s">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="2" t="s">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="2" t="s">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" s="2" t="s">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B135" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="2" t="s">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="2" t="s">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B139" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B140" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B142" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="2" t="s">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="2" t="s">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="2" t="s">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="2" t="s">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B148" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B149" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B150" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="2" t="s">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
-        <v>208</v>
-      </c>
-      <c r="B152" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="2" t="s">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="2" t="s">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="2" t="s">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B156" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="2" t="s">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="2" t="s">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="2" t="s">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B161" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B162" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" s="2" t="s">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" s="2" t="s">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" s="2" t="s">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" s="2" t="s">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B167" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B168" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
-        <v>203</v>
-      </c>
-      <c r="B169" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" s="2" t="s">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" s="2" t="s">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B172" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B173" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" s="2" t="s">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" s="2" t="s">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" s="2" t="s">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B178" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" s="2" t="s">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" s="2" t="s">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" s="2" t="s">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B182" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" s="2" t="s">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A184" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B184" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A185" s="2" t="s">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A186" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B186" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A187" s="2" t="s">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B188" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A189" t="s">
-        <v>204</v>
-      </c>
-      <c r="B189" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A190" s="2" t="s">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A191" s="2" t="s">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A192" s="2" t="s">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A193" s="2" t="s">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A194" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A195" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B195" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A196" s="2" t="s">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" s="2" t="s">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A198" s="2" t="s">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A199" s="2" t="s">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A200" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A201" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B201" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A202" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B202" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A203" s="2" t="s">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A204" s="2" t="s">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A205" s="2" t="s">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A206" s="2" t="s">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A207" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A208" s="2" t="s">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A209" s="2" t="s">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A210" s="2" t="s">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A211" s="2" t="s">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A212" s="2" t="s">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
-        <v>216</v>
-      </c>
-      <c r="B213" t="s">
-        <v>213</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B212">
-    <sortCondition ref="A2:A212"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B213">
+    <sortCondition ref="B2:B213"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>